<commit_message>
Crear mas repuestos | Ordenamiento (ASC, DESC, IDLE) | Buscador mejorado | Manejo stock poco mejorado
</commit_message>
<xml_diff>
--- a/src/Plantilla_excel.xlsx
+++ b/src/Plantilla_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franco\Desktop\actual\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Colegio\Planilla (PPs)\SoftwareDML-Testing\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F54D7A-2748-4003-B667-85A30C10D4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADC7583-FC48-44B4-AEB3-B6B60A811B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="0" windowWidth="19185" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,53 +717,53 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1204,15 +1204,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="61"/>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="68"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="6"/>
       <c r="E3" s="5"/>
     </row>
@@ -1340,34 +1340,34 @@
       <c r="E16" s="67"/>
     </row>
     <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="70"/>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="70"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="70"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
@@ -1377,15 +1377,15 @@
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="69" t="s">
+      <c r="A22" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69" t="s">
+      <c r="B22" s="77"/>
+      <c r="C22" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
@@ -1440,48 +1440,48 @@
       <c r="E26" s="18"/>
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="71"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="71"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
+      <c r="A30" s="78"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="71"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="71"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
+      <c r="A32" s="78"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="71"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
@@ -1491,13 +1491,13 @@
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="72" t="s">
+      <c r="A35" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
@@ -1506,67 +1506,67 @@
       <c r="B36" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="73" t="s">
+      <c r="C36" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
     </row>
     <row r="37" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="22"/>
       <c r="B37" s="23"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
     </row>
     <row r="38" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="20"/>
       <c r="B38" s="23"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
     </row>
     <row r="39" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="20"/>
       <c r="B39" s="23"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
     </row>
     <row r="40" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
       <c r="B40" s="23"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
     </row>
     <row r="41" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="20"/>
       <c r="B41" s="24"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
     </row>
     <row r="42" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="20"/>
       <c r="B42" s="24"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="20"/>
       <c r="B43" s="25"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="20"/>
       <c r="B44" s="25"/>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="42"/>
@@ -1576,12 +1576,12 @@
       <c r="E45" s="42"/>
     </row>
     <row r="46" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="79" t="s">
+      <c r="A46" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="80"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="81"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="72"/>
       <c r="E46" s="42"/>
     </row>
     <row r="47" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1632,16 +1632,16 @@
     <row r="52" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
       <c r="B52" s="19"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
       <c r="E52" s="26"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="82" t="s">
+      <c r="A53" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="83"/>
-      <c r="C53" s="83"/>
+      <c r="B53" s="74"/>
+      <c r="C53" s="74"/>
       <c r="D53" s="52" t="s">
         <v>25</v>
       </c>
@@ -1656,26 +1656,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E33"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="A46:D46"/>
     <mergeCell ref="A53:C53"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A29:E33"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>